<commit_message>
Relatorio do BC replicado
</commit_message>
<xml_diff>
--- a/ipca_servicos.xlsx
+++ b/ipca_servicos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/amandars1_al_insper_edu_br/Documents/Insper/7° Semestre/Econolab/entrega_final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Insper\7\EconoLab\econolab_entrega_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{199023E7-87A7-4F3B-82A4-CB0CB69C5260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102C0E25-45FB-4954-8E26-E73E5C00D685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{151E0960-DD07-4EDE-AEA8-2E96081844AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{151E0960-DD07-4EDE-AEA8-2E96081844AF}"/>
   </bookViews>
   <sheets>
     <sheet name="ipca_servicos" sheetId="1" r:id="rId1"/>
@@ -896,12 +896,12 @@
   <dimension ref="A1:B306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>36526</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>36557</v>
       </c>
@@ -925,7 +925,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>36586</v>
       </c>
@@ -933,7 +933,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>36617</v>
       </c>
@@ -941,7 +941,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>36647</v>
       </c>
@@ -949,7 +949,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36678</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>36708</v>
       </c>
@@ -965,7 +965,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>36739</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>36770</v>
       </c>
@@ -981,7 +981,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>36800</v>
       </c>
@@ -989,7 +989,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>36831</v>
       </c>
@@ -997,7 +997,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>36861</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>36892</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>36923</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>36951</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>36982</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>37012</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>37043</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>37073</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>37104</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>37135</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>37165</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>37196</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>37226</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>37257</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>37288</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>37316</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>37347</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>37377</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>37408</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>37438</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>37469</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>37500</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>37530</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>37561</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>37591</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37622</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37653</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>37681</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>37712</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>37742</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>37773</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>37803</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>37834</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>37865</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>37895</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>37926</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>37956</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>37987</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>38018</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>38047</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>38078</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>38108</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>38139</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>38169</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>38200</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>38231</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>38261</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>38292</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>38322</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>38353</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>38384</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>38412</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>38443</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>38473</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>38504</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>38534</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>38565</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>38596</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>38626</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>38657</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>38687</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>38718</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>38749</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>38777</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>38808</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>38838</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>38869</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>38899</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>38930</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>38961</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>38991</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>39022</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>39052</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>39083</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>39114</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>39142</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>39173</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>39203</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>39234</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>39264</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>39295</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>39326</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>39356</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>39387</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>39417</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>39448</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>39479</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>39508</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>39539</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>39569</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>39600</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>39630</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>39661</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>39692</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>39722</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>39753</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>39783</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>39814</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>39845</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>39873</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>39904</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>39934</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>39965</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>39995</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>40026</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>40057</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>40087</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>40118</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>40148</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>40179</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>40210</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>40238</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>40269</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>40299</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>40330</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>40360</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>40391</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>40422</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>40452</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>40483</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>40513</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>40544</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>40575</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>40603</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>40634</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>40664</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>40695</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>40725</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>40756</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>40787</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>40817</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>40848</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>40878</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>40909</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>40940</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>40969</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>41000</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>41030</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>41061</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>41091</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>41122</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>41153</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>41183</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>41214</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>41244</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>41275</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>41306</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>41334</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>41365</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>41395</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>41426</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>41456</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>41487</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>41518</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>41548</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>41579</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>41609</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>41640</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>41671</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>41699</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>41730</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>41760</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>41791</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>41821</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>41852</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>41883</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>41913</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>41944</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>41974</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>42005</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>42036</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>42064</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>42095</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>42125</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>42156</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>42186</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>42217</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>42248</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>42278</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>42309</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>42339</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>42370</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>42401</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>42430</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>42461</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>42491</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>42522</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>42552</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>42583</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>42614</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>42644</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>42675</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>42705</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>42736</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>42767</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>42795</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>42826</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>42856</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>42887</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>42917</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>42948</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>42979</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>43009</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>43040</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>43070</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>43101</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>43132</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>43160</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>43191</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>43221</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>43252</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>43282</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>43313</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>43344</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>43374</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>43405</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>43435</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>43466</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>43497</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>43525</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>43556</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>43586</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>43617</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>43647</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>43678</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>43709</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>43739</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>43770</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>43800</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>43831</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>43862</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>43891</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>43922</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>43952</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>43983</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>-0.26</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>44013</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>44044</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>44075</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>44105</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>44136</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>44166</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>44197</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>44228</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>44256</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>44287</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>44317</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>44348</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>44378</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>44409</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>44440</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>44470</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>44501</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>44531</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>44562</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>44593</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>44621</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>44652</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>44682</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>44713</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>44743</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>44774</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>44805</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>44835</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>44866</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>44896</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>44927</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>44958</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>44986</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>45017</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>45047</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>45078</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>45108</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>45139</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>45170</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>45200</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <v>45231</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>45261</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>45292</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>45323</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>45352</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>45383</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>45413</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>45444</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>45474</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>45505</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>45536</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>45566</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>45597</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>45627</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>45658</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>45689</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>45717</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>45748</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>2</v>
       </c>

</xml_diff>